<commit_message>
Start blacklisting weird names
</commit_message>
<xml_diff>
--- a/pipeline/painter_counts_ordered.xlsx
+++ b/pipeline/painter_counts_ordered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelwaugh/Desktop/Desktop - Samuel’s MacBook Pro/artefact-context/pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F45836-4D79-034C-A7BF-031D5174D085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EFD1F9-9ECF-B74A-B251-400158D6073C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9454,8 +9454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3021"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9482,6 +9482,9 @@
       <c r="B2">
         <v>2514</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -9490,6 +9493,9 @@
       <c r="B3">
         <v>2504</v>
       </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -9498,6 +9504,9 @@
       <c r="B4">
         <v>2178</v>
       </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -9506,6 +9515,9 @@
       <c r="B5">
         <v>1354</v>
       </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -9514,6 +9526,9 @@
       <c r="B6">
         <v>634</v>
       </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -9522,6 +9537,9 @@
       <c r="B7">
         <v>613</v>
       </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -9530,6 +9548,9 @@
       <c r="B8">
         <v>599</v>
       </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -9538,6 +9559,9 @@
       <c r="B9">
         <v>536</v>
       </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
@@ -9595,7 +9619,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -9603,15 +9627,18 @@
         <v>359</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
         <v>358</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -9619,7 +9646,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -9627,7 +9654,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -9635,7 +9662,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -9643,7 +9670,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -9651,7 +9678,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -9659,7 +9686,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -9667,7 +9694,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -9675,7 +9702,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -9683,7 +9710,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -9691,7 +9718,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -9699,7 +9726,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -9707,7 +9734,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -9715,7 +9742,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Blacklist for bad names
</commit_message>
<xml_diff>
--- a/pipeline/painter_counts_ordered.xlsx
+++ b/pipeline/painter_counts_ordered.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelwaugh/Desktop/Desktop - Samuel’s MacBook Pro/artefact-context/pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EFD1F9-9ECF-B74A-B251-400158D6073C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E07D63-5373-8E48-BEB0-9023192431BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30240" windowHeight="19640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="10000" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -9454,8 +9454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3021"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A270" workbookViewId="0">
+      <selection activeCell="A297" sqref="A297"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9626,6 +9626,9 @@
       <c r="B17">
         <v>359</v>
       </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -9669,6 +9672,9 @@
       <c r="B22">
         <v>323</v>
       </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -9685,6 +9691,9 @@
       <c r="B24">
         <v>300</v>
       </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -9750,7 +9759,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -9758,7 +9767,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -9766,7 +9775,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -9774,7 +9783,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -9782,7 +9791,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -9790,7 +9799,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -9798,7 +9807,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -9806,7 +9815,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -9814,7 +9823,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -9822,7 +9831,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -9830,7 +9839,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -9838,7 +9847,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -9846,7 +9855,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -9854,23 +9863,29 @@
         <v>191</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46">
         <v>189</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47">
         <v>186</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -9878,7 +9893,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -9886,15 +9901,18 @@
         <v>178</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50">
         <v>177</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -9902,7 +9920,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -9910,7 +9928,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -9918,7 +9936,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -9926,7 +9944,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -9934,7 +9952,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -9942,7 +9960,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -9950,7 +9968,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -9958,7 +9976,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -9966,7 +9984,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -9974,7 +9992,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -9982,7 +10000,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -9990,7 +10008,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -9998,7 +10016,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>64</v>
       </c>

</xml_diff>